<commit_message>
added columns data aswell
</commit_message>
<xml_diff>
--- a/incrOrderCuda/experiment_data.xlsx
+++ b/incrOrderCuda/experiment_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gil-t\Desktop\dev\High-Performance-Systems\incrOrderCuda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B864A36-E70F-4A7F-8378-261E5BE5064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FC49A7-3FAF-4B0F-A242-5436B6FEACC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49D1E07E-1220-4C40-87CD-2DA84B69BA7B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rows" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Blocks</t>
   </si>
@@ -112,6 +113,1947 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Exec_Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t> / </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>#Blocks</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Rows!$B$1:$L$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Rows!$B$8:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0186234000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.47430339999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24025819999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1409802</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.13308840000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11812719999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.2434000000000016E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.1640799999999986E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.1843200000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.8125000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.12412000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-13D8-42CA-B1AF-5B18475BE026}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="845839439"/>
+        <c:axId val="845844015"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="845839439"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="845844015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="845844015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="845839439"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$L$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.16888719999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16033059999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1558446</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15187300000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14705499999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1428266</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15186459999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15329280000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.15536240000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.20759699999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.23549999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6AA9-440E-9775-6C93C36F54FC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="848678159"/>
+        <c:axId val="848681903"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="848678159"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="848681903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="848681903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.25"/>
+          <c:min val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="848678159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92EECDD4-9C66-CA83-7D41-C3FD4694A31A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E4D660D-0853-03D0-4991-FA7E025E26BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,8 +2355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09502B0F-D16E-4263-AE93-E71F124C5A32}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" activeCellId="1" sqref="B8 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,47 +2597,47 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <f>AVERAGE(B2,B3,B4,B5,B6)</f>
+        <f t="shared" ref="B8:L8" si="0">AVERAGE(B2,B3,B4,B5,B6)</f>
         <v>1.0186234000000001</v>
       </c>
       <c r="C8">
-        <f>AVERAGE(C2,C3,C4,C5,C6)</f>
+        <f t="shared" si="0"/>
         <v>0.47430339999999999</v>
       </c>
       <c r="D8">
-        <f>AVERAGE(D2,D3,D4,D5,D6)</f>
+        <f t="shared" si="0"/>
         <v>0.24025819999999998</v>
       </c>
       <c r="E8">
-        <f>AVERAGE(E2,E3,E4,E5,E6)</f>
+        <f t="shared" si="0"/>
         <v>0.1409802</v>
       </c>
       <c r="F8">
-        <f>AVERAGE(F2,F3,F4,F5,F6)</f>
+        <f t="shared" si="0"/>
         <v>0.13308840000000002</v>
       </c>
       <c r="G8">
-        <f>AVERAGE(G2,G3,G4,G5,G6)</f>
+        <f t="shared" si="0"/>
         <v>0.11812719999999999</v>
       </c>
       <c r="H8">
-        <f>AVERAGE(H2,H3,H4,H5,H6)</f>
+        <f t="shared" si="0"/>
         <v>9.2434000000000016E-2</v>
       </c>
       <c r="I8">
-        <f>AVERAGE(I2,I3,I4,I5,I6)</f>
+        <f t="shared" si="0"/>
         <v>8.1640799999999986E-2</v>
       </c>
       <c r="J8">
-        <f>AVERAGE(J2,J3,J4,J5,J6)</f>
+        <f t="shared" si="0"/>
         <v>8.1843200000000005E-2</v>
       </c>
       <c r="K8">
-        <f>AVERAGE(K2,K3,K4,K5,K6)</f>
+        <f t="shared" si="0"/>
         <v>9.8125000000000004E-2</v>
       </c>
       <c r="L8">
-        <f>AVERAGE(L2,L3,L4,L5,L6)</f>
+        <f t="shared" si="0"/>
         <v>0.12412000000000001</v>
       </c>
     </row>
@@ -704,52 +2646,396 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <f>_xlfn.STDEV.P(B2,B3,B4,B5,B6,B8)</f>
+        <f t="shared" ref="B9:L9" si="1">_xlfn.STDEV.P(B2,B3,B4,B5,B6,B8)</f>
         <v>6.038591447238928E-4</v>
       </c>
       <c r="C9">
-        <f>_xlfn.STDEV.P(C2,C3,C4,C5,C6,C8)</f>
+        <f t="shared" si="1"/>
         <v>5.0074264847323462E-4</v>
       </c>
       <c r="D9">
-        <f>_xlfn.STDEV.P(D2,D3,D4,D5,D6,D8)</f>
+        <f t="shared" si="1"/>
         <v>4.6483057845484425E-4</v>
       </c>
       <c r="E9">
-        <f>_xlfn.STDEV.P(E2,E3,E4,E5,E6,E8)</f>
+        <f t="shared" si="1"/>
         <v>3.8667617804393335E-4</v>
       </c>
       <c r="F9">
-        <f>_xlfn.STDEV.P(F2,F3,F4,F5,F6,F8)</f>
+        <f t="shared" si="1"/>
         <v>1.3007382519169303E-4</v>
       </c>
       <c r="G9">
-        <f>_xlfn.STDEV.P(G2,G3,G4,G5,G6,G8)</f>
+        <f t="shared" si="1"/>
         <v>8.0310646865779144E-5</v>
       </c>
       <c r="H9">
-        <f>_xlfn.STDEV.P(H2,H3,H4,H5,H6,H8)</f>
+        <f t="shared" si="1"/>
         <v>5.3500778810530538E-5</v>
       </c>
       <c r="I9">
-        <f>_xlfn.STDEV.P(I2,I3,I4,I5,I6,I8)</f>
+        <f t="shared" si="1"/>
         <v>2.6766894976196066E-5</v>
       </c>
       <c r="J9">
-        <f>_xlfn.STDEV.P(J2,J3,J4,J5,J6,J8)</f>
+        <f t="shared" si="1"/>
         <v>2.3504609477010101E-5</v>
       </c>
       <c r="K9">
-        <f>_xlfn.STDEV.P(K2,K3,K4,K5,K6,K8)</f>
+        <f t="shared" si="1"/>
         <v>3.4753896664019307E-4</v>
       </c>
       <c r="L9">
-        <f>_xlfn.STDEV.P(L2,L3,L4,L5,L6,L8)</f>
+        <f t="shared" si="1"/>
         <v>4.2190046219457808E-4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0647DE69-B0AE-40A5-81F0-1B46B4B80A0B}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>8</v>
+      </c>
+      <c r="F1">
+        <v>16</v>
+      </c>
+      <c r="G1">
+        <v>32</v>
+      </c>
+      <c r="H1">
+        <v>64</v>
+      </c>
+      <c r="I1">
+        <v>128</v>
+      </c>
+      <c r="J1">
+        <v>256</v>
+      </c>
+      <c r="K1">
+        <v>512</v>
+      </c>
+      <c r="L1">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.169515</v>
+      </c>
+      <c r="C2">
+        <v>0.16017899999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.157551</v>
+      </c>
+      <c r="E2">
+        <v>0.15129799999999999</v>
+      </c>
+      <c r="F2">
+        <v>0.146985</v>
+      </c>
+      <c r="G2">
+        <v>0.143016</v>
+      </c>
+      <c r="H2">
+        <v>0.15277299999999999</v>
+      </c>
+      <c r="I2">
+        <v>0.153086</v>
+      </c>
+      <c r="J2">
+        <v>0.15584000000000001</v>
+      </c>
+      <c r="K2">
+        <v>0.20894299999999999</v>
+      </c>
+      <c r="L2">
+        <v>0.2374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0.16842499999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.15989400000000001</v>
+      </c>
+      <c r="D3">
+        <v>0.154697</v>
+      </c>
+      <c r="E3">
+        <v>0.15190999999999999</v>
+      </c>
+      <c r="F3">
+        <v>0.14627100000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.14296500000000001</v>
+      </c>
+      <c r="H3">
+        <v>0.150842</v>
+      </c>
+      <c r="I3">
+        <v>0.15318699999999999</v>
+      </c>
+      <c r="J3">
+        <v>0.15514800000000001</v>
+      </c>
+      <c r="K3">
+        <v>0.206818</v>
+      </c>
+      <c r="L3">
+        <v>0.23630000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0.169266</v>
+      </c>
+      <c r="C4">
+        <v>0.160716</v>
+      </c>
+      <c r="D4">
+        <v>0.15462899999999999</v>
+      </c>
+      <c r="E4">
+        <v>0.15194299999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.14879600000000001</v>
+      </c>
+      <c r="G4">
+        <v>0.14302899999999999</v>
+      </c>
+      <c r="H4">
+        <v>0.152669</v>
+      </c>
+      <c r="I4">
+        <v>0.15262899999999999</v>
+      </c>
+      <c r="J4">
+        <v>0.15546099999999999</v>
+      </c>
+      <c r="K4">
+        <v>0.20791899999999999</v>
+      </c>
+      <c r="L4">
+        <v>0.2364</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.16775399999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.159917</v>
+      </c>
+      <c r="D5">
+        <v>0.15704599999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.151781</v>
+      </c>
+      <c r="F5">
+        <v>0.14666899999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.14302599999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.15204500000000001</v>
+      </c>
+      <c r="I5">
+        <v>0.153442</v>
+      </c>
+      <c r="J5">
+        <v>0.155144</v>
+      </c>
+      <c r="K5">
+        <v>0.20598900000000001</v>
+      </c>
+      <c r="L5">
+        <v>0.2329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.16947599999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.16094700000000001</v>
+      </c>
+      <c r="D6">
+        <v>0.15529999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.15243300000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.14655399999999999</v>
+      </c>
+      <c r="G6">
+        <v>0.142097</v>
+      </c>
+      <c r="H6">
+        <v>0.15099399999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.15412000000000001</v>
+      </c>
+      <c r="J6">
+        <v>0.155219</v>
+      </c>
+      <c r="K6">
+        <v>0.208316</v>
+      </c>
+      <c r="L6">
+        <v>0.23449999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(B2,B3,B4,B5,B6)</f>
+        <v>0.16888719999999999</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:L8" si="0">AVERAGE(C2,C3,C4,C5,C6)</f>
+        <v>0.16033059999999999</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.1558446</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.15187300000000001</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.14705499999999999</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>0.1428266</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.15186459999999999</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0.15329280000000001</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0.15536240000000001</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>0.20759699999999998</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>0.23549999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f>_xlfn.STDEV.P(B2,B3,B4,B5,B6,B8)</f>
+        <v>6.3008978196233052E-4</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:L9" si="1">_xlfn.STDEV.P(C2,C3,C4,C5,C6,C8)</f>
+        <v>3.901173327773752E-4</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>1.1140333029133376E-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>3.3140056326647635E-4</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>8.2164814042671129E-4</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>3.3368378244479524E-4</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>7.4256865002503302E-4</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>4.4742053298137569E-4</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>2.422303311588647E-4</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>9.6823430359942219E-4</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>1.4617341299520503E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>